<commit_message>
Julia conversion branch checkpoint
</commit_message>
<xml_diff>
--- a/Misc/julia optimization.xlsx
+++ b/Misc/julia optimization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Documents\GitHub\VPC\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BFBF40F-07B0-4613-80A7-DC94531752E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BF6C84-62C7-4F26-99D3-A6B327F6A040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27945" windowHeight="16440" xr2:uid="{9C247AB6-2951-4DCB-9C2F-C80228F519CB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>BLAS</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>tmap</t>
+  </si>
+  <si>
+    <t>Sun+ser</t>
+  </si>
+  <si>
+    <t>Sun+tm</t>
   </si>
 </sst>
 </file>
@@ -425,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5D8A88-1B80-4518-B26B-9C81EA2A7CD4}">
-  <dimension ref="C1:H31"/>
+  <dimension ref="C1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>1</v>
       </c>
@@ -473,7 +479,7 @@
         <v>3.6059999999999999</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>1</v>
       </c>
@@ -481,47 +487,121 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5">
         <v>9.6660000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6">
         <v>7.2389999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>3.9340000000000002</v>
+      </c>
+      <c r="O6">
+        <v>1.732</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
         <v>5.1660000000000004</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>6.6959999999999997</v>
+      </c>
+      <c r="O7">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>5</v>
       </c>
       <c r="E8">
         <v>4.1989999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>6.9930000000000003</v>
+      </c>
+      <c r="O8">
+        <v>1.9690000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>6</v>
       </c>
       <c r="E9">
         <v>4.47</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>4.2149999999999999</v>
+      </c>
+      <c r="O9">
+        <v>1.972</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>4.0609999999999999</v>
+      </c>
+      <c r="O10">
+        <v>2.3679999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>0</v>
       </c>
@@ -534,8 +614,20 @@
       <c r="F11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>4.1360000000000001</v>
+      </c>
+      <c r="O11">
+        <v>2.427</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>2</v>
       </c>
@@ -548,8 +640,20 @@
       <c r="F12">
         <v>4.024</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>4.024</v>
+      </c>
+      <c r="O12">
+        <v>2.665</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>3</v>
       </c>
@@ -562,8 +666,20 @@
       <c r="F13">
         <v>3.7839999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>3.6709999999999998</v>
+      </c>
+      <c r="O13">
+        <v>2.786</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>4</v>
       </c>
@@ -577,7 +693,7 @@
         <v>3.7890000000000001</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>5</v>
       </c>
@@ -591,7 +707,7 @@
         <v>3.5529999999999999</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>6</v>
       </c>
@@ -605,7 +721,7 @@
         <v>3.9740000000000002</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>0</v>
       </c>
@@ -618,8 +734,14 @@
       <c r="F17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>1</v>
       </c>
@@ -632,8 +754,22 @@
       <c r="F18">
         <v>2.4820000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>2.0209999999999999</v>
+      </c>
+      <c r="H18">
+        <v>0.877</v>
+      </c>
+      <c r="I18">
+        <f>G$26/H18</f>
+        <v>2.1083238312428736</v>
+      </c>
+      <c r="J18">
+        <f>I18/D18</f>
+        <v>1.0541619156214368</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>1</v>
       </c>
@@ -647,7 +783,7 @@
         <v>1.9610000000000001</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
@@ -660,8 +796,22 @@
       <c r="F20">
         <v>1.756</v>
       </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>1.861</v>
+      </c>
+      <c r="H20">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I19:I25" si="0">G$26/H20</f>
+        <v>4.7654639175257731</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ref="J19:J25" si="1">I20/D20</f>
+        <v>1.1913659793814433</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>1</v>
       </c>
@@ -675,7 +825,7 @@
         <v>1.6579999999999999</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>1</v>
       </c>
@@ -688,138 +838,98 @@
       <c r="F22">
         <v>1.5249999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>1.8320000000000001</v>
+      </c>
+      <c r="H22">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>4.8403141361256541</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>0.80671902268760898</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="H23">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>7.0304182509505697</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0.87880228136882121</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>3.9340000000000002</v>
-      </c>
-      <c r="F24">
-        <v>1.732</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>1.8</v>
+      </c>
+      <c r="H24">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>7.6404958677685952</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0.76404958677685952</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>4</v>
-      </c>
-      <c r="E25">
-        <v>6.6959999999999997</v>
-      </c>
-      <c r="F25">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="E26">
-        <v>6.9930000000000003</v>
-      </c>
-      <c r="F26">
-        <v>1.9690000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <v>4.2149999999999999</v>
-      </c>
-      <c r="F27">
-        <v>1.972</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28">
-        <v>3</v>
-      </c>
-      <c r="E28">
-        <v>4.0609999999999999</v>
-      </c>
-      <c r="F28">
-        <v>2.3679999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="E29">
-        <v>4.1360000000000001</v>
-      </c>
-      <c r="F29">
-        <v>2.427</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30">
-        <v>4.024</v>
-      </c>
-      <c r="F30">
-        <v>2.665</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31">
-        <v>3.6709999999999998</v>
-      </c>
-      <c r="F31">
-        <v>2.786</v>
+        <v>12</v>
+      </c>
+      <c r="G25">
+        <v>1.7849999999999999</v>
+      </c>
+      <c r="H25">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>8.1096491228070171</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0.67580409356725146</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f>AVERAGE(G18:G25)</f>
+        <v>1.849</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C24:F31">
-    <sortCondition ref="F24:F31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L6:O13">
+    <sortCondition ref="O6:O13"/>
   </sortState>
-  <conditionalFormatting sqref="F12:F16 F18:F22 F24:F31">
+  <conditionalFormatting sqref="O6:O13 F12:F16 F18:F22">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>